<commit_message>
updated acm "about" tab
</commit_message>
<xml_diff>
--- a/great_debate/US_ACM analysis.xlsx
+++ b/great_debate/US_ACM analysis.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\great_debate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1010048A-29CE-43A4-84D7-BF83328B668F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CF2DDA-9258-4494-9E3B-EA24602524E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="2690" windowWidth="25300" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20300" yWindow="7860" windowWidth="25300" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -475,6 +486,12 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" kern="1200" baseline="0"/>
+            <a:t>Data extraction limited to county with 2019 population of 100,000 or more (the 596 largest counties in America)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -500,7 +517,11 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t> </a:t>
+            <a:t> rates on 1/4/2022 by</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0"/>
+            <a:t> County for </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -556,7 +577,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t> </a:t>
+            <a:t> and population by County</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-US"/>
@@ -853,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>